<commit_message>
Actualizar Logica de Devoluciones
</commit_message>
<xml_diff>
--- a/Documentacion/Product backlog/Product Backlog v1.3/Historias Técnicas versión 1.3.xlsx
+++ b/Documentacion/Product backlog/Product Backlog v1.3/Historias Técnicas versión 1.3.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Saeteros\Desktop\Proyecto_E-commerce\Documentacion\Product backlog\Product Backlog v1.2\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Saeteros\Desktop\Proyecto_E-commerce\Documentacion\Product backlog\Product Backlog v1.3\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D1D994B9-DA97-42C4-BE97-FF08E86DDDC3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{258146CD-8F2D-42E3-9825-865F2B00659E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -21,7 +21,6 @@
     <definedName name="_xlnm.Print_Area" localSheetId="1">Instructivo!$A$1:$D$13</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -39,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="316" uniqueCount="227">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="309" uniqueCount="224">
   <si>
     <t>Columna</t>
   </si>
@@ -650,15 +649,6 @@
   </si>
   <si>
     <t>HT-048</t>
-  </si>
-  <si>
-    <t>Documentar la funcionalidad final</t>
-  </si>
-  <si>
-    <t>Crear documentación que describa el sistema completo, sus funciones y flujos.</t>
-  </si>
-  <si>
-    <t>- La documentación debe ser clara y comprensible para usuarios finales y administradores.</t>
   </si>
   <si>
     <t>HT-049</t>
@@ -1109,31 +1099,22 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1162,6 +1143,15 @@
     </xf>
     <xf numFmtId="0" fontId="6" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1499,10 +1489,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9D1DBEB7-C3D2-4473-9B85-4CF26F3AA489}">
-  <dimension ref="B1:AJ130"/>
+  <dimension ref="B1:AJ129"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A48" zoomScale="70" zoomScaleNormal="70" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="H59" sqref="H59"/>
+    <sheetView tabSelected="1" topLeftCell="A39" zoomScale="50" zoomScaleNormal="50" zoomScaleSheetLayoutView="100" workbookViewId="0">
+      <selection activeCell="C50" sqref="C50:C51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15"/>
@@ -1522,16 +1512,16 @@
   <sheetData>
     <row r="1" spans="2:36" ht="15.75" thickBot="1"/>
     <row r="2" spans="2:36" ht="36" customHeight="1">
-      <c r="B2" s="28" t="s">
+      <c r="B2" s="25" t="s">
         <v>26</v>
       </c>
-      <c r="C2" s="29"/>
-      <c r="D2" s="29"/>
-      <c r="E2" s="29"/>
-      <c r="F2" s="29"/>
-      <c r="G2" s="29"/>
-      <c r="H2" s="29"/>
-      <c r="I2" s="30"/>
+      <c r="C2" s="26"/>
+      <c r="D2" s="26"/>
+      <c r="E2" s="26"/>
+      <c r="F2" s="26"/>
+      <c r="G2" s="26"/>
+      <c r="H2" s="26"/>
+      <c r="I2" s="27"/>
       <c r="K2" s="6"/>
       <c r="L2" s="6"/>
       <c r="M2" s="6"/>
@@ -1560,14 +1550,14 @@
       <c r="AJ2" s="6"/>
     </row>
     <row r="3" spans="2:36" ht="21" customHeight="1">
-      <c r="B3" s="31"/>
-      <c r="C3" s="32"/>
-      <c r="D3" s="32"/>
-      <c r="E3" s="32"/>
-      <c r="F3" s="32"/>
-      <c r="G3" s="32"/>
-      <c r="H3" s="32"/>
-      <c r="I3" s="33"/>
+      <c r="B3" s="28"/>
+      <c r="C3" s="29"/>
+      <c r="D3" s="29"/>
+      <c r="E3" s="29"/>
+      <c r="F3" s="29"/>
+      <c r="G3" s="29"/>
+      <c r="H3" s="29"/>
+      <c r="I3" s="30"/>
       <c r="K3" s="6"/>
       <c r="L3" s="6"/>
       <c r="M3" s="6"/>
@@ -1596,14 +1586,14 @@
       <c r="AJ3" s="6"/>
     </row>
     <row r="4" spans="2:36" ht="15.75" customHeight="1" thickBot="1">
-      <c r="B4" s="34"/>
-      <c r="C4" s="35"/>
-      <c r="D4" s="35"/>
-      <c r="E4" s="35"/>
-      <c r="F4" s="35"/>
-      <c r="G4" s="35"/>
-      <c r="H4" s="35"/>
-      <c r="I4" s="36"/>
+      <c r="B4" s="31"/>
+      <c r="C4" s="32"/>
+      <c r="D4" s="32"/>
+      <c r="E4" s="32"/>
+      <c r="F4" s="32"/>
+      <c r="G4" s="32"/>
+      <c r="H4" s="32"/>
+      <c r="I4" s="33"/>
       <c r="K4" s="6"/>
       <c r="L4" s="6"/>
       <c r="M4" s="6"/>
@@ -1684,22 +1674,22 @@
       <c r="AJ5" s="6"/>
     </row>
     <row r="6" spans="2:36" ht="51.75" customHeight="1" thickBot="1">
-      <c r="B6" s="25" t="s">
+      <c r="B6" s="19" t="s">
         <v>27</v>
       </c>
-      <c r="C6" s="26" t="s">
+      <c r="C6" s="21" t="s">
         <v>39</v>
       </c>
-      <c r="D6" s="26" t="s">
+      <c r="D6" s="21" t="s">
         <v>112</v>
       </c>
-      <c r="E6" s="27" t="s">
+      <c r="E6" s="23" t="s">
         <v>40</v>
       </c>
-      <c r="F6" s="27" t="s">
+      <c r="F6" s="23" t="s">
         <v>20</v>
       </c>
-      <c r="G6" s="27" t="s">
+      <c r="G6" s="23" t="s">
         <v>41</v>
       </c>
       <c r="H6" s="12" t="s">
@@ -1739,9 +1729,9 @@
       <c r="B7" s="20"/>
       <c r="C7" s="22"/>
       <c r="D7" s="22"/>
-      <c r="E7" s="19"/>
-      <c r="F7" s="19"/>
-      <c r="G7" s="19"/>
+      <c r="E7" s="24"/>
+      <c r="F7" s="24"/>
+      <c r="G7" s="24"/>
       <c r="H7" s="15" t="s">
         <v>114</v>
       </c>
@@ -1785,13 +1775,13 @@
       <c r="D8" s="22" t="s">
         <v>43</v>
       </c>
-      <c r="E8" s="19" t="s">
+      <c r="E8" s="24" t="s">
         <v>44</v>
       </c>
-      <c r="F8" s="19" t="s">
+      <c r="F8" s="24" t="s">
         <v>20</v>
       </c>
-      <c r="G8" s="19" t="s">
+      <c r="G8" s="24" t="s">
         <v>27</v>
       </c>
       <c r="H8" s="15" t="s">
@@ -1831,9 +1821,9 @@
       <c r="B9" s="20"/>
       <c r="C9" s="22"/>
       <c r="D9" s="22"/>
-      <c r="E9" s="19"/>
-      <c r="F9" s="19"/>
-      <c r="G9" s="19"/>
+      <c r="E9" s="24"/>
+      <c r="F9" s="24"/>
+      <c r="G9" s="24"/>
       <c r="H9" s="15" t="s">
         <v>116</v>
       </c>
@@ -1877,13 +1867,13 @@
       <c r="D10" s="22" t="s">
         <v>46</v>
       </c>
-      <c r="E10" s="19" t="s">
+      <c r="E10" s="24" t="s">
         <v>44</v>
       </c>
-      <c r="F10" s="19" t="s">
+      <c r="F10" s="24" t="s">
         <v>20</v>
       </c>
-      <c r="G10" s="19" t="s">
+      <c r="G10" s="24" t="s">
         <v>27</v>
       </c>
       <c r="H10" s="15" t="s">
@@ -1923,9 +1913,9 @@
       <c r="B11" s="20"/>
       <c r="C11" s="22"/>
       <c r="D11" s="22"/>
-      <c r="E11" s="19"/>
-      <c r="F11" s="19"/>
-      <c r="G11" s="19"/>
+      <c r="E11" s="24"/>
+      <c r="F11" s="24"/>
+      <c r="G11" s="24"/>
       <c r="H11" s="15" t="s">
         <v>118</v>
       </c>
@@ -1969,13 +1959,13 @@
       <c r="D12" s="22" t="s">
         <v>48</v>
       </c>
-      <c r="E12" s="19" t="s">
+      <c r="E12" s="24" t="s">
         <v>44</v>
       </c>
-      <c r="F12" s="19" t="s">
+      <c r="F12" s="24" t="s">
         <v>20</v>
       </c>
-      <c r="G12" s="19" t="s">
+      <c r="G12" s="24" t="s">
         <v>27</v>
       </c>
       <c r="H12" s="15" t="s">
@@ -2015,9 +2005,9 @@
       <c r="B13" s="20"/>
       <c r="C13" s="22"/>
       <c r="D13" s="22"/>
-      <c r="E13" s="19"/>
-      <c r="F13" s="19"/>
-      <c r="G13" s="19"/>
+      <c r="E13" s="24"/>
+      <c r="F13" s="24"/>
+      <c r="G13" s="24"/>
       <c r="H13" s="15" t="s">
         <v>120</v>
       </c>
@@ -2113,13 +2103,13 @@
       <c r="D15" s="22" t="s">
         <v>52</v>
       </c>
-      <c r="E15" s="19" t="s">
+      <c r="E15" s="24" t="s">
         <v>53</v>
       </c>
-      <c r="F15" s="19" t="s">
+      <c r="F15" s="24" t="s">
         <v>20</v>
       </c>
-      <c r="G15" s="19" t="s">
+      <c r="G15" s="24" t="s">
         <v>29</v>
       </c>
       <c r="H15" s="15" t="s">
@@ -2159,9 +2149,9 @@
       <c r="B16" s="20"/>
       <c r="C16" s="22"/>
       <c r="D16" s="22"/>
-      <c r="E16" s="19"/>
-      <c r="F16" s="19"/>
-      <c r="G16" s="19"/>
+      <c r="E16" s="24"/>
+      <c r="F16" s="24"/>
+      <c r="G16" s="24"/>
       <c r="H16" s="15" t="s">
         <v>122</v>
       </c>
@@ -2205,13 +2195,13 @@
       <c r="D17" s="22" t="s">
         <v>56</v>
       </c>
-      <c r="E17" s="19" t="s">
+      <c r="E17" s="24" t="s">
         <v>53</v>
       </c>
-      <c r="F17" s="19" t="s">
+      <c r="F17" s="24" t="s">
         <v>20</v>
       </c>
-      <c r="G17" s="19" t="s">
+      <c r="G17" s="24" t="s">
         <v>30</v>
       </c>
       <c r="H17" s="15" t="s">
@@ -2251,9 +2241,9 @@
       <c r="B18" s="20"/>
       <c r="C18" s="22"/>
       <c r="D18" s="22"/>
-      <c r="E18" s="19"/>
-      <c r="F18" s="19"/>
-      <c r="G18" s="19"/>
+      <c r="E18" s="24"/>
+      <c r="F18" s="24"/>
+      <c r="G18" s="24"/>
       <c r="H18" s="15" t="s">
         <v>124</v>
       </c>
@@ -2349,13 +2339,13 @@
       <c r="D20" s="22" t="s">
         <v>60</v>
       </c>
-      <c r="E20" s="19" t="s">
+      <c r="E20" s="24" t="s">
         <v>53</v>
       </c>
-      <c r="F20" s="19" t="s">
+      <c r="F20" s="24" t="s">
         <v>20</v>
       </c>
-      <c r="G20" s="19" t="s">
+      <c r="G20" s="24" t="s">
         <v>28</v>
       </c>
       <c r="H20" s="15" t="s">
@@ -2395,9 +2385,9 @@
       <c r="B21" s="20"/>
       <c r="C21" s="22"/>
       <c r="D21" s="22"/>
-      <c r="E21" s="19"/>
-      <c r="F21" s="19"/>
-      <c r="G21" s="19"/>
+      <c r="E21" s="24"/>
+      <c r="F21" s="24"/>
+      <c r="G21" s="24"/>
       <c r="H21" s="15" t="s">
         <v>126</v>
       </c>
@@ -2545,13 +2535,13 @@
       <c r="D24" s="22" t="s">
         <v>67</v>
       </c>
-      <c r="E24" s="19" t="s">
+      <c r="E24" s="24" t="s">
         <v>40</v>
       </c>
-      <c r="F24" s="19" t="s">
+      <c r="F24" s="24" t="s">
         <v>20</v>
       </c>
-      <c r="G24" s="19" t="s">
+      <c r="G24" s="24" t="s">
         <v>68</v>
       </c>
       <c r="H24" s="15" t="s">
@@ -2591,9 +2581,9 @@
       <c r="B25" s="20"/>
       <c r="C25" s="22"/>
       <c r="D25" s="22"/>
-      <c r="E25" s="19"/>
-      <c r="F25" s="19"/>
-      <c r="G25" s="19"/>
+      <c r="E25" s="24"/>
+      <c r="F25" s="24"/>
+      <c r="G25" s="24"/>
       <c r="H25" s="15" t="s">
         <v>128</v>
       </c>
@@ -2689,13 +2679,13 @@
       <c r="D27" s="22" t="s">
         <v>141</v>
       </c>
-      <c r="E27" s="19" t="s">
+      <c r="E27" s="24" t="s">
         <v>44</v>
       </c>
-      <c r="F27" s="19" t="s">
+      <c r="F27" s="24" t="s">
         <v>107</v>
       </c>
-      <c r="G27" s="19" t="s">
+      <c r="G27" s="24" t="s">
         <v>142</v>
       </c>
       <c r="H27" s="15" t="s">
@@ -2735,9 +2725,9 @@
       <c r="B28" s="20"/>
       <c r="C28" s="22"/>
       <c r="D28" s="22"/>
-      <c r="E28" s="19"/>
-      <c r="F28" s="19"/>
-      <c r="G28" s="19"/>
+      <c r="E28" s="24"/>
+      <c r="F28" s="24"/>
+      <c r="G28" s="24"/>
       <c r="H28" s="15" t="s">
         <v>144</v>
       </c>
@@ -2781,13 +2771,13 @@
       <c r="D29" s="22" t="s">
         <v>147</v>
       </c>
-      <c r="E29" s="19" t="s">
+      <c r="E29" s="24" t="s">
         <v>44</v>
       </c>
-      <c r="F29" s="19" t="s">
+      <c r="F29" s="24" t="s">
         <v>107</v>
       </c>
-      <c r="G29" s="19" t="s">
+      <c r="G29" s="24" t="s">
         <v>148</v>
       </c>
       <c r="H29" s="15" t="s">
@@ -2827,9 +2817,9 @@
       <c r="B30" s="20"/>
       <c r="C30" s="22"/>
       <c r="D30" s="22"/>
-      <c r="E30" s="19"/>
-      <c r="F30" s="19"/>
-      <c r="G30" s="19"/>
+      <c r="E30" s="24"/>
+      <c r="F30" s="24"/>
+      <c r="G30" s="24"/>
       <c r="H30" s="15" t="s">
         <v>150</v>
       </c>
@@ -2873,13 +2863,13 @@
       <c r="D31" s="22" t="s">
         <v>153</v>
       </c>
-      <c r="E31" s="19" t="s">
+      <c r="E31" s="24" t="s">
         <v>53</v>
       </c>
-      <c r="F31" s="19" t="s">
+      <c r="F31" s="24" t="s">
         <v>107</v>
       </c>
-      <c r="G31" s="19" t="s">
+      <c r="G31" s="24" t="s">
         <v>154</v>
       </c>
       <c r="H31" s="15" t="s">
@@ -2919,9 +2909,9 @@
       <c r="B32" s="20"/>
       <c r="C32" s="22"/>
       <c r="D32" s="22"/>
-      <c r="E32" s="19"/>
-      <c r="F32" s="19"/>
-      <c r="G32" s="19"/>
+      <c r="E32" s="24"/>
+      <c r="F32" s="24"/>
+      <c r="G32" s="24"/>
       <c r="H32" s="15" t="s">
         <v>156</v>
       </c>
@@ -2965,13 +2955,13 @@
       <c r="D33" s="22" t="s">
         <v>159</v>
       </c>
-      <c r="E33" s="19" t="s">
+      <c r="E33" s="24" t="s">
         <v>53</v>
       </c>
-      <c r="F33" s="19" t="s">
+      <c r="F33" s="24" t="s">
         <v>107</v>
       </c>
-      <c r="G33" s="19" t="s">
+      <c r="G33" s="24" t="s">
         <v>160</v>
       </c>
       <c r="H33" s="15" t="s">
@@ -3011,9 +3001,9 @@
       <c r="B34" s="20"/>
       <c r="C34" s="22"/>
       <c r="D34" s="22"/>
-      <c r="E34" s="19"/>
-      <c r="F34" s="19"/>
-      <c r="G34" s="19"/>
+      <c r="E34" s="24"/>
+      <c r="F34" s="24"/>
+      <c r="G34" s="24"/>
       <c r="H34" s="15" t="s">
         <v>162</v>
       </c>
@@ -3070,7 +3060,7 @@
         <v>167</v>
       </c>
       <c r="I35" s="13" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K35" s="6"/>
       <c r="L35" s="6"/>
@@ -3109,20 +3099,20 @@
       <c r="D36" s="22" t="s">
         <v>170</v>
       </c>
-      <c r="E36" s="19" t="s">
+      <c r="E36" s="24" t="s">
         <v>97</v>
       </c>
-      <c r="F36" s="19" t="s">
+      <c r="F36" s="24" t="s">
         <v>20</v>
       </c>
-      <c r="G36" s="19" t="s">
+      <c r="G36" s="24" t="s">
         <v>171</v>
       </c>
       <c r="H36" s="15" t="s">
         <v>172</v>
       </c>
       <c r="I36" s="13" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K36" s="6"/>
       <c r="L36" s="6"/>
@@ -3155,14 +3145,14 @@
       <c r="B37" s="20"/>
       <c r="C37" s="22"/>
       <c r="D37" s="22"/>
-      <c r="E37" s="19"/>
-      <c r="F37" s="19"/>
-      <c r="G37" s="19"/>
+      <c r="E37" s="24"/>
+      <c r="F37" s="24"/>
+      <c r="G37" s="24"/>
       <c r="H37" s="15" t="s">
         <v>173</v>
       </c>
       <c r="I37" s="13" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K37" s="6"/>
       <c r="L37" s="6"/>
@@ -3305,13 +3295,13 @@
       <c r="D40" s="22" t="s">
         <v>91</v>
       </c>
-      <c r="E40" s="19" t="s">
+      <c r="E40" s="24" t="s">
         <v>53</v>
       </c>
-      <c r="F40" s="19" t="s">
+      <c r="F40" s="24" t="s">
         <v>20</v>
       </c>
-      <c r="G40" s="19" t="s">
+      <c r="G40" s="24" t="s">
         <v>92</v>
       </c>
       <c r="H40" s="15" t="s">
@@ -3351,9 +3341,9 @@
       <c r="B41" s="20"/>
       <c r="C41" s="22"/>
       <c r="D41" s="22"/>
-      <c r="E41" s="19"/>
-      <c r="F41" s="19"/>
-      <c r="G41" s="19"/>
+      <c r="E41" s="24"/>
+      <c r="F41" s="24"/>
+      <c r="G41" s="24"/>
       <c r="H41" s="15" t="s">
         <v>130</v>
       </c>
@@ -3397,13 +3387,13 @@
       <c r="D42" s="22" t="s">
         <v>95</v>
       </c>
-      <c r="E42" s="19" t="s">
+      <c r="E42" s="24" t="s">
         <v>53</v>
       </c>
-      <c r="F42" s="19" t="s">
+      <c r="F42" s="24" t="s">
         <v>20</v>
       </c>
-      <c r="G42" s="19" t="s">
+      <c r="G42" s="24" t="s">
         <v>96</v>
       </c>
       <c r="H42" s="15" t="s">
@@ -3443,9 +3433,9 @@
       <c r="B43" s="20"/>
       <c r="C43" s="22"/>
       <c r="D43" s="22"/>
-      <c r="E43" s="19"/>
-      <c r="F43" s="19"/>
-      <c r="G43" s="19"/>
+      <c r="E43" s="24"/>
+      <c r="F43" s="24"/>
+      <c r="G43" s="24"/>
       <c r="H43" s="15" t="s">
         <v>132</v>
       </c>
@@ -3489,13 +3479,13 @@
       <c r="D44" s="22" t="s">
         <v>100</v>
       </c>
-      <c r="E44" s="19" t="s">
+      <c r="E44" s="24" t="s">
         <v>40</v>
       </c>
-      <c r="F44" s="19" t="s">
+      <c r="F44" s="24" t="s">
         <v>20</v>
       </c>
-      <c r="G44" s="19" t="s">
+      <c r="G44" s="24" t="s">
         <v>101</v>
       </c>
       <c r="H44" s="15" t="s">
@@ -3535,9 +3525,9 @@
       <c r="B45" s="20"/>
       <c r="C45" s="22"/>
       <c r="D45" s="22"/>
-      <c r="E45" s="19"/>
-      <c r="F45" s="19"/>
-      <c r="G45" s="19"/>
+      <c r="E45" s="24"/>
+      <c r="F45" s="24"/>
+      <c r="G45" s="24"/>
       <c r="H45" s="15" t="s">
         <v>134</v>
       </c>
@@ -3581,13 +3571,13 @@
       <c r="D46" s="22" t="s">
         <v>104</v>
       </c>
-      <c r="E46" s="19" t="s">
+      <c r="E46" s="24" t="s">
         <v>53</v>
       </c>
-      <c r="F46" s="19" t="s">
+      <c r="F46" s="24" t="s">
         <v>20</v>
       </c>
-      <c r="G46" s="19" t="s">
+      <c r="G46" s="24" t="s">
         <v>105</v>
       </c>
       <c r="H46" s="15" t="s">
@@ -3627,9 +3617,9 @@
       <c r="B47" s="20"/>
       <c r="C47" s="22"/>
       <c r="D47" s="22"/>
-      <c r="E47" s="19"/>
-      <c r="F47" s="19"/>
-      <c r="G47" s="19"/>
+      <c r="E47" s="24"/>
+      <c r="F47" s="24"/>
+      <c r="G47" s="24"/>
       <c r="H47" s="15" t="s">
         <v>136</v>
       </c>
@@ -3673,13 +3663,13 @@
       <c r="D48" s="22" t="s">
         <v>177</v>
       </c>
-      <c r="E48" s="19" t="s">
+      <c r="E48" s="24" t="s">
         <v>54</v>
       </c>
-      <c r="F48" s="19" t="s">
+      <c r="F48" s="24" t="s">
         <v>107</v>
       </c>
-      <c r="G48" s="19" t="s">
+      <c r="G48" s="24" t="s">
         <v>108</v>
       </c>
       <c r="H48" s="15" t="s">
@@ -3719,9 +3709,9 @@
       <c r="B49" s="20"/>
       <c r="C49" s="22"/>
       <c r="D49" s="22"/>
-      <c r="E49" s="19"/>
-      <c r="F49" s="19"/>
-      <c r="G49" s="19"/>
+      <c r="E49" s="24"/>
+      <c r="F49" s="24"/>
+      <c r="G49" s="24"/>
       <c r="H49" s="15" t="s">
         <v>138</v>
       </c>
@@ -3765,13 +3755,13 @@
       <c r="D50" s="22" t="s">
         <v>180</v>
       </c>
-      <c r="E50" s="19" t="s">
+      <c r="E50" s="24" t="s">
         <v>53</v>
       </c>
-      <c r="F50" s="19" t="s">
+      <c r="F50" s="24" t="s">
         <v>20</v>
       </c>
-      <c r="G50" s="19" t="s">
+      <c r="G50" s="24" t="s">
         <v>181</v>
       </c>
       <c r="H50" s="18" t="s">
@@ -3811,9 +3801,9 @@
       <c r="B51" s="20"/>
       <c r="C51" s="22"/>
       <c r="D51" s="22"/>
-      <c r="E51" s="19"/>
-      <c r="F51" s="19"/>
-      <c r="G51" s="19"/>
+      <c r="E51" s="24"/>
+      <c r="F51" s="24"/>
+      <c r="G51" s="24"/>
       <c r="H51" s="15" t="s">
         <v>183</v>
       </c>
@@ -3857,13 +3847,13 @@
       <c r="D52" s="22" t="s">
         <v>184</v>
       </c>
-      <c r="E52" s="19" t="s">
+      <c r="E52" s="24" t="s">
         <v>54</v>
       </c>
-      <c r="F52" s="19" t="s">
+      <c r="F52" s="24" t="s">
         <v>20</v>
       </c>
-      <c r="G52" s="19" t="s">
+      <c r="G52" s="24" t="s">
         <v>109</v>
       </c>
       <c r="H52" s="15" t="s">
@@ -3903,9 +3893,9 @@
       <c r="B53" s="20"/>
       <c r="C53" s="22"/>
       <c r="D53" s="22"/>
-      <c r="E53" s="19"/>
-      <c r="F53" s="19"/>
-      <c r="G53" s="19"/>
+      <c r="E53" s="24"/>
+      <c r="F53" s="24"/>
+      <c r="G53" s="24"/>
       <c r="H53" s="15" t="s">
         <v>175</v>
       </c>
@@ -3949,13 +3939,13 @@
       <c r="D54" s="22" t="s">
         <v>187</v>
       </c>
-      <c r="E54" s="19" t="s">
+      <c r="E54" s="24" t="s">
         <v>53</v>
       </c>
-      <c r="F54" s="19" t="s">
+      <c r="F54" s="24" t="s">
         <v>20</v>
       </c>
-      <c r="G54" s="19" t="s">
+      <c r="G54" s="24" t="s">
         <v>41</v>
       </c>
       <c r="H54" s="15" t="s">
@@ -3995,9 +3985,9 @@
       <c r="B55" s="20"/>
       <c r="C55" s="22"/>
       <c r="D55" s="22"/>
-      <c r="E55" s="19"/>
-      <c r="F55" s="19"/>
-      <c r="G55" s="19"/>
+      <c r="E55" s="24"/>
+      <c r="F55" s="24"/>
+      <c r="G55" s="24"/>
       <c r="H55" s="15" t="s">
         <v>189</v>
       </c>
@@ -4041,13 +4031,13 @@
       <c r="D56" s="22" t="s">
         <v>192</v>
       </c>
-      <c r="E56" s="19" t="s">
+      <c r="E56" s="24" t="s">
         <v>40</v>
       </c>
-      <c r="F56" s="19" t="s">
+      <c r="F56" s="24" t="s">
         <v>107</v>
       </c>
-      <c r="G56" s="19" t="s">
+      <c r="G56" s="24" t="s">
         <v>171</v>
       </c>
       <c r="H56" s="15" t="s">
@@ -4087,9 +4077,9 @@
       <c r="B57" s="20"/>
       <c r="C57" s="22"/>
       <c r="D57" s="22"/>
-      <c r="E57" s="19"/>
-      <c r="F57" s="19"/>
-      <c r="G57" s="19"/>
+      <c r="E57" s="24"/>
+      <c r="F57" s="24"/>
+      <c r="G57" s="24"/>
       <c r="H57" s="15" t="s">
         <v>194</v>
       </c>
@@ -4133,13 +4123,13 @@
       <c r="D58" s="22" t="s">
         <v>197</v>
       </c>
-      <c r="E58" s="19" t="s">
+      <c r="E58" s="24" t="s">
         <v>54</v>
       </c>
-      <c r="F58" s="19" t="s">
+      <c r="F58" s="24" t="s">
         <v>20</v>
       </c>
-      <c r="G58" s="19" t="s">
+      <c r="G58" s="24" t="s">
         <v>109</v>
       </c>
       <c r="H58" s="15" t="s">
@@ -4179,9 +4169,9 @@
       <c r="B59" s="20"/>
       <c r="C59" s="22"/>
       <c r="D59" s="22"/>
-      <c r="E59" s="19"/>
-      <c r="F59" s="19"/>
-      <c r="G59" s="19"/>
+      <c r="E59" s="24"/>
+      <c r="F59" s="24"/>
+      <c r="G59" s="24"/>
       <c r="H59" s="15" t="s">
         <v>199</v>
       </c>
@@ -4215,27 +4205,27 @@
       <c r="AI59" s="6"/>
       <c r="AJ59" s="6"/>
     </row>
-    <row r="60" spans="2:36" thickBot="1">
-      <c r="B60" s="14" t="s">
-        <v>200</v>
-      </c>
-      <c r="C60" s="15" t="s">
+    <row r="60" spans="2:36" ht="18.75" thickBot="1">
+      <c r="B60" s="20" t="s">
         <v>201</v>
       </c>
-      <c r="D60" s="15" t="s">
+      <c r="C60" s="22" t="s">
         <v>202</v>
       </c>
-      <c r="E60" s="16" t="s">
+      <c r="D60" s="22" t="s">
+        <v>203</v>
+      </c>
+      <c r="E60" s="24" t="s">
         <v>40</v>
       </c>
-      <c r="F60" s="16" t="s">
+      <c r="F60" s="24" t="s">
         <v>20</v>
       </c>
-      <c r="G60" s="16" t="s">
+      <c r="G60" s="24" t="s">
         <v>109</v>
       </c>
       <c r="H60" s="15" t="s">
-        <v>203</v>
+        <v>204</v>
       </c>
       <c r="I60" s="13" t="b">
         <v>0</v>
@@ -4268,26 +4258,14 @@
       <c r="AJ60" s="6"/>
     </row>
     <row r="61" spans="2:36" ht="18.75" thickBot="1">
-      <c r="B61" s="20" t="s">
-        <v>204</v>
-      </c>
-      <c r="C61" s="22" t="s">
+      <c r="B61" s="20"/>
+      <c r="C61" s="22"/>
+      <c r="D61" s="22"/>
+      <c r="E61" s="24"/>
+      <c r="F61" s="24"/>
+      <c r="G61" s="24"/>
+      <c r="H61" s="15" t="s">
         <v>205</v>
-      </c>
-      <c r="D61" s="22" t="s">
-        <v>206</v>
-      </c>
-      <c r="E61" s="19" t="s">
-        <v>40</v>
-      </c>
-      <c r="F61" s="19" t="s">
-        <v>20</v>
-      </c>
-      <c r="G61" s="19" t="s">
-        <v>109</v>
-      </c>
-      <c r="H61" s="15" t="s">
-        <v>207</v>
       </c>
       <c r="I61" s="13" t="b">
         <v>0</v>
@@ -4320,14 +4298,26 @@
       <c r="AJ61" s="6"/>
     </row>
     <row r="62" spans="2:36" ht="18.75" thickBot="1">
-      <c r="B62" s="20"/>
-      <c r="C62" s="22"/>
-      <c r="D62" s="22"/>
-      <c r="E62" s="19"/>
-      <c r="F62" s="19"/>
-      <c r="G62" s="19"/>
-      <c r="H62" s="15" t="s">
+      <c r="B62" s="20" t="s">
+        <v>206</v>
+      </c>
+      <c r="C62" s="22" t="s">
+        <v>207</v>
+      </c>
+      <c r="D62" s="22" t="s">
         <v>208</v>
+      </c>
+      <c r="E62" s="24" t="s">
+        <v>54</v>
+      </c>
+      <c r="F62" s="24" t="s">
+        <v>20</v>
+      </c>
+      <c r="G62" s="24" t="s">
+        <v>201</v>
+      </c>
+      <c r="H62" s="18" t="s">
+        <v>209</v>
       </c>
       <c r="I62" s="13" t="b">
         <v>0</v>
@@ -4360,26 +4350,14 @@
       <c r="AJ62" s="6"/>
     </row>
     <row r="63" spans="2:36" ht="18.75" thickBot="1">
-      <c r="B63" s="20" t="s">
-        <v>209</v>
-      </c>
-      <c r="C63" s="22" t="s">
+      <c r="B63" s="20"/>
+      <c r="C63" s="22"/>
+      <c r="D63" s="22"/>
+      <c r="E63" s="24"/>
+      <c r="F63" s="24"/>
+      <c r="G63" s="24"/>
+      <c r="H63" s="18" t="s">
         <v>210</v>
-      </c>
-      <c r="D63" s="22" t="s">
-        <v>211</v>
-      </c>
-      <c r="E63" s="19" t="s">
-        <v>54</v>
-      </c>
-      <c r="F63" s="19" t="s">
-        <v>20</v>
-      </c>
-      <c r="G63" s="19" t="s">
-        <v>204</v>
-      </c>
-      <c r="H63" s="18" t="s">
-        <v>212</v>
       </c>
       <c r="I63" s="13" t="b">
         <v>0</v>
@@ -4412,14 +4390,26 @@
       <c r="AJ63" s="6"/>
     </row>
     <row r="64" spans="2:36" ht="18.75" thickBot="1">
-      <c r="B64" s="20"/>
-      <c r="C64" s="22"/>
-      <c r="D64" s="22"/>
-      <c r="E64" s="19"/>
-      <c r="F64" s="19"/>
-      <c r="G64" s="19"/>
-      <c r="H64" s="18" t="s">
+      <c r="B64" s="20" t="s">
+        <v>211</v>
+      </c>
+      <c r="C64" s="22" t="s">
+        <v>212</v>
+      </c>
+      <c r="D64" s="22" t="s">
         <v>213</v>
+      </c>
+      <c r="E64" s="24" t="s">
+        <v>53</v>
+      </c>
+      <c r="F64" s="24" t="s">
+        <v>107</v>
+      </c>
+      <c r="G64" s="24" t="s">
+        <v>200</v>
+      </c>
+      <c r="H64" s="15" t="s">
+        <v>214</v>
       </c>
       <c r="I64" s="13" t="b">
         <v>0</v>
@@ -4452,26 +4442,14 @@
       <c r="AJ64" s="6"/>
     </row>
     <row r="65" spans="2:36" ht="18.75" thickBot="1">
-      <c r="B65" s="20" t="s">
-        <v>214</v>
-      </c>
-      <c r="C65" s="22" t="s">
+      <c r="B65" s="20"/>
+      <c r="C65" s="22"/>
+      <c r="D65" s="22"/>
+      <c r="E65" s="24"/>
+      <c r="F65" s="24"/>
+      <c r="G65" s="24"/>
+      <c r="H65" s="15" t="s">
         <v>215</v>
-      </c>
-      <c r="D65" s="22" t="s">
-        <v>216</v>
-      </c>
-      <c r="E65" s="19" t="s">
-        <v>53</v>
-      </c>
-      <c r="F65" s="19" t="s">
-        <v>107</v>
-      </c>
-      <c r="G65" s="19" t="s">
-        <v>200</v>
-      </c>
-      <c r="H65" s="15" t="s">
-        <v>217</v>
       </c>
       <c r="I65" s="13" t="b">
         <v>0</v>
@@ -4504,14 +4482,26 @@
       <c r="AJ65" s="6"/>
     </row>
     <row r="66" spans="2:36" ht="18.75" thickBot="1">
-      <c r="B66" s="20"/>
-      <c r="C66" s="22"/>
-      <c r="D66" s="22"/>
-      <c r="E66" s="19"/>
-      <c r="F66" s="19"/>
-      <c r="G66" s="19"/>
+      <c r="B66" s="20" t="s">
+        <v>216</v>
+      </c>
+      <c r="C66" s="22" t="s">
+        <v>217</v>
+      </c>
+      <c r="D66" s="22" t="s">
+        <v>218</v>
+      </c>
+      <c r="E66" s="24" t="s">
+        <v>40</v>
+      </c>
+      <c r="F66" s="24" t="s">
+        <v>20</v>
+      </c>
+      <c r="G66" s="24" t="s">
+        <v>109</v>
+      </c>
       <c r="H66" s="15" t="s">
-        <v>218</v>
+        <v>219</v>
       </c>
       <c r="I66" s="13" t="b">
         <v>0</v>
@@ -4543,27 +4533,15 @@
       <c r="AI66" s="6"/>
       <c r="AJ66" s="6"/>
     </row>
-    <row r="67" spans="2:36" ht="18.75" thickBot="1">
-      <c r="B67" s="20" t="s">
-        <v>219</v>
-      </c>
-      <c r="C67" s="22" t="s">
+    <row r="67" spans="2:36" ht="36.75" thickBot="1">
+      <c r="B67" s="20"/>
+      <c r="C67" s="22"/>
+      <c r="D67" s="22"/>
+      <c r="E67" s="24"/>
+      <c r="F67" s="24"/>
+      <c r="G67" s="24"/>
+      <c r="H67" s="15" t="s">
         <v>220</v>
-      </c>
-      <c r="D67" s="22" t="s">
-        <v>221</v>
-      </c>
-      <c r="E67" s="19" t="s">
-        <v>40</v>
-      </c>
-      <c r="F67" s="19" t="s">
-        <v>20</v>
-      </c>
-      <c r="G67" s="19" t="s">
-        <v>109</v>
-      </c>
-      <c r="H67" s="15" t="s">
-        <v>222</v>
       </c>
       <c r="I67" s="13" t="b">
         <v>0</v>
@@ -4596,14 +4574,26 @@
       <c r="AJ67" s="6"/>
     </row>
     <row r="68" spans="2:36" ht="36.75" thickBot="1">
-      <c r="B68" s="20"/>
-      <c r="C68" s="22"/>
-      <c r="D68" s="22"/>
-      <c r="E68" s="19"/>
-      <c r="F68" s="19"/>
-      <c r="G68" s="19"/>
+      <c r="B68" s="20" t="s">
+        <v>86</v>
+      </c>
+      <c r="C68" s="22" t="s">
+        <v>87</v>
+      </c>
+      <c r="D68" s="22" t="s">
+        <v>221</v>
+      </c>
+      <c r="E68" s="24" t="s">
+        <v>54</v>
+      </c>
+      <c r="F68" s="24" t="s">
+        <v>20</v>
+      </c>
+      <c r="G68" s="24" t="s">
+        <v>88</v>
+      </c>
       <c r="H68" s="15" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="I68" s="13" t="b">
         <v>0</v>
@@ -4635,27 +4625,15 @@
       <c r="AI68" s="6"/>
       <c r="AJ68" s="6"/>
     </row>
-    <row r="69" spans="2:36" ht="36.75" thickBot="1">
-      <c r="B69" s="20" t="s">
-        <v>86</v>
-      </c>
-      <c r="C69" s="22" t="s">
-        <v>87</v>
-      </c>
-      <c r="D69" s="22" t="s">
-        <v>224</v>
-      </c>
-      <c r="E69" s="19" t="s">
-        <v>54</v>
-      </c>
-      <c r="F69" s="19" t="s">
-        <v>20</v>
-      </c>
-      <c r="G69" s="19" t="s">
-        <v>88</v>
-      </c>
-      <c r="H69" s="15" t="s">
-        <v>225</v>
+    <row r="69" spans="2:36" ht="18.75" thickBot="1">
+      <c r="B69" s="34"/>
+      <c r="C69" s="35"/>
+      <c r="D69" s="35"/>
+      <c r="E69" s="36"/>
+      <c r="F69" s="36"/>
+      <c r="G69" s="36"/>
+      <c r="H69" s="17" t="s">
+        <v>223</v>
       </c>
       <c r="I69" s="13" t="b">
         <v>0</v>
@@ -4687,19 +4665,7 @@
       <c r="AI69" s="6"/>
       <c r="AJ69" s="6"/>
     </row>
-    <row r="70" spans="2:36" ht="18.75" thickBot="1">
-      <c r="B70" s="21"/>
-      <c r="C70" s="23"/>
-      <c r="D70" s="23"/>
-      <c r="E70" s="24"/>
-      <c r="F70" s="24"/>
-      <c r="G70" s="24"/>
-      <c r="H70" s="17" t="s">
-        <v>226</v>
-      </c>
-      <c r="I70" s="13" t="b">
-        <v>0</v>
-      </c>
+    <row r="70" spans="2:36">
       <c r="K70" s="6"/>
       <c r="L70" s="6"/>
       <c r="M70" s="6"/>
@@ -6379,36 +6345,158 @@
       <c r="AI129" s="6"/>
       <c r="AJ129" s="6"/>
     </row>
-    <row r="130" spans="11:36">
-      <c r="K130" s="6"/>
-      <c r="L130" s="6"/>
-      <c r="M130" s="6"/>
-      <c r="N130" s="6"/>
-      <c r="O130" s="6"/>
-      <c r="P130" s="6"/>
-      <c r="Q130" s="6"/>
-      <c r="R130" s="6"/>
-      <c r="S130" s="6"/>
-      <c r="T130" s="6"/>
-      <c r="U130" s="6"/>
-      <c r="V130" s="6"/>
-      <c r="W130" s="6"/>
-      <c r="X130" s="6"/>
-      <c r="Y130" s="6"/>
-      <c r="Z130" s="6"/>
-      <c r="AA130" s="6"/>
-      <c r="AB130" s="6"/>
-      <c r="AC130" s="6"/>
-      <c r="AD130" s="6"/>
-      <c r="AE130" s="6"/>
-      <c r="AF130" s="6"/>
-      <c r="AG130" s="6"/>
-      <c r="AH130" s="6"/>
-      <c r="AI130" s="6"/>
-      <c r="AJ130" s="6"/>
-    </row>
   </sheetData>
   <mergeCells count="169">
+    <mergeCell ref="G66:G67"/>
+    <mergeCell ref="B68:B69"/>
+    <mergeCell ref="C68:C69"/>
+    <mergeCell ref="D68:D69"/>
+    <mergeCell ref="E68:E69"/>
+    <mergeCell ref="F68:F69"/>
+    <mergeCell ref="G68:G69"/>
+    <mergeCell ref="B66:B67"/>
+    <mergeCell ref="C66:C67"/>
+    <mergeCell ref="D66:D67"/>
+    <mergeCell ref="E66:E67"/>
+    <mergeCell ref="F66:F67"/>
+    <mergeCell ref="G62:G63"/>
+    <mergeCell ref="B64:B65"/>
+    <mergeCell ref="C64:C65"/>
+    <mergeCell ref="D64:D65"/>
+    <mergeCell ref="E64:E65"/>
+    <mergeCell ref="F64:F65"/>
+    <mergeCell ref="G64:G65"/>
+    <mergeCell ref="B62:B63"/>
+    <mergeCell ref="C62:C63"/>
+    <mergeCell ref="D62:D63"/>
+    <mergeCell ref="E62:E63"/>
+    <mergeCell ref="F62:F63"/>
+    <mergeCell ref="G58:G59"/>
+    <mergeCell ref="B60:B61"/>
+    <mergeCell ref="C60:C61"/>
+    <mergeCell ref="D60:D61"/>
+    <mergeCell ref="E60:E61"/>
+    <mergeCell ref="F60:F61"/>
+    <mergeCell ref="G60:G61"/>
+    <mergeCell ref="B58:B59"/>
+    <mergeCell ref="C58:C59"/>
+    <mergeCell ref="D58:D59"/>
+    <mergeCell ref="E58:E59"/>
+    <mergeCell ref="F58:F59"/>
+    <mergeCell ref="G54:G55"/>
+    <mergeCell ref="B56:B57"/>
+    <mergeCell ref="C56:C57"/>
+    <mergeCell ref="D56:D57"/>
+    <mergeCell ref="E56:E57"/>
+    <mergeCell ref="F56:F57"/>
+    <mergeCell ref="G56:G57"/>
+    <mergeCell ref="B54:B55"/>
+    <mergeCell ref="C54:C55"/>
+    <mergeCell ref="D54:D55"/>
+    <mergeCell ref="E54:E55"/>
+    <mergeCell ref="F54:F55"/>
+    <mergeCell ref="G50:G51"/>
+    <mergeCell ref="B50:B51"/>
+    <mergeCell ref="C50:C51"/>
+    <mergeCell ref="D50:D51"/>
+    <mergeCell ref="E50:E51"/>
+    <mergeCell ref="F50:F51"/>
+    <mergeCell ref="G52:G53"/>
+    <mergeCell ref="B52:B53"/>
+    <mergeCell ref="C52:C53"/>
+    <mergeCell ref="D52:D53"/>
+    <mergeCell ref="E52:E53"/>
+    <mergeCell ref="F52:F53"/>
+    <mergeCell ref="B44:B45"/>
+    <mergeCell ref="C44:C45"/>
+    <mergeCell ref="D44:D45"/>
+    <mergeCell ref="E44:E45"/>
+    <mergeCell ref="F44:F45"/>
+    <mergeCell ref="G44:G45"/>
+    <mergeCell ref="G46:G47"/>
+    <mergeCell ref="B48:B49"/>
+    <mergeCell ref="C48:C49"/>
+    <mergeCell ref="D48:D49"/>
+    <mergeCell ref="E48:E49"/>
+    <mergeCell ref="F48:F49"/>
+    <mergeCell ref="G48:G49"/>
+    <mergeCell ref="B46:B47"/>
+    <mergeCell ref="C46:C47"/>
+    <mergeCell ref="D46:D47"/>
+    <mergeCell ref="E46:E47"/>
+    <mergeCell ref="F46:F47"/>
+    <mergeCell ref="B40:B41"/>
+    <mergeCell ref="C40:C41"/>
+    <mergeCell ref="D40:D41"/>
+    <mergeCell ref="E40:E41"/>
+    <mergeCell ref="F40:F41"/>
+    <mergeCell ref="G40:G41"/>
+    <mergeCell ref="B42:B43"/>
+    <mergeCell ref="C42:C43"/>
+    <mergeCell ref="D42:D43"/>
+    <mergeCell ref="E42:E43"/>
+    <mergeCell ref="F42:F43"/>
+    <mergeCell ref="G42:G43"/>
+    <mergeCell ref="B36:B37"/>
+    <mergeCell ref="C36:C37"/>
+    <mergeCell ref="D36:D37"/>
+    <mergeCell ref="E36:E37"/>
+    <mergeCell ref="F36:F37"/>
+    <mergeCell ref="G36:G37"/>
+    <mergeCell ref="G31:G32"/>
+    <mergeCell ref="B33:B34"/>
+    <mergeCell ref="C33:C34"/>
+    <mergeCell ref="D33:D34"/>
+    <mergeCell ref="E33:E34"/>
+    <mergeCell ref="F33:F34"/>
+    <mergeCell ref="G33:G34"/>
+    <mergeCell ref="B31:B32"/>
+    <mergeCell ref="C31:C32"/>
+    <mergeCell ref="D31:D32"/>
+    <mergeCell ref="E31:E32"/>
+    <mergeCell ref="F31:F32"/>
+    <mergeCell ref="G24:G25"/>
+    <mergeCell ref="B29:B30"/>
+    <mergeCell ref="C29:C30"/>
+    <mergeCell ref="D29:D30"/>
+    <mergeCell ref="E29:E30"/>
+    <mergeCell ref="F29:F30"/>
+    <mergeCell ref="G29:G30"/>
+    <mergeCell ref="B27:B28"/>
+    <mergeCell ref="C27:C28"/>
+    <mergeCell ref="D27:D28"/>
+    <mergeCell ref="E27:E28"/>
+    <mergeCell ref="F27:F28"/>
+    <mergeCell ref="G27:G28"/>
+    <mergeCell ref="B24:B25"/>
+    <mergeCell ref="C24:C25"/>
+    <mergeCell ref="D24:D25"/>
+    <mergeCell ref="E24:E25"/>
+    <mergeCell ref="F24:F25"/>
+    <mergeCell ref="G17:G18"/>
+    <mergeCell ref="B20:B21"/>
+    <mergeCell ref="C20:C21"/>
+    <mergeCell ref="D20:D21"/>
+    <mergeCell ref="E20:E21"/>
+    <mergeCell ref="F20:F21"/>
+    <mergeCell ref="G20:G21"/>
+    <mergeCell ref="B17:B18"/>
+    <mergeCell ref="C17:C18"/>
+    <mergeCell ref="D17:D18"/>
+    <mergeCell ref="E17:E18"/>
+    <mergeCell ref="F17:F18"/>
+    <mergeCell ref="G12:G13"/>
+    <mergeCell ref="B15:B16"/>
+    <mergeCell ref="C15:C16"/>
+    <mergeCell ref="D15:D16"/>
+    <mergeCell ref="E15:E16"/>
+    <mergeCell ref="F15:F16"/>
+    <mergeCell ref="G15:G16"/>
+    <mergeCell ref="B12:B13"/>
+    <mergeCell ref="C12:C13"/>
+    <mergeCell ref="D12:D13"/>
+    <mergeCell ref="E12:E13"/>
+    <mergeCell ref="F12:F13"/>
     <mergeCell ref="B6:B7"/>
     <mergeCell ref="C6:C7"/>
     <mergeCell ref="D6:D7"/>
@@ -6428,158 +6516,8 @@
     <mergeCell ref="D8:D9"/>
     <mergeCell ref="E8:E9"/>
     <mergeCell ref="F8:F9"/>
-    <mergeCell ref="G12:G13"/>
-    <mergeCell ref="B15:B16"/>
-    <mergeCell ref="C15:C16"/>
-    <mergeCell ref="D15:D16"/>
-    <mergeCell ref="E15:E16"/>
-    <mergeCell ref="F15:F16"/>
-    <mergeCell ref="G15:G16"/>
-    <mergeCell ref="B12:B13"/>
-    <mergeCell ref="C12:C13"/>
-    <mergeCell ref="D12:D13"/>
-    <mergeCell ref="E12:E13"/>
-    <mergeCell ref="F12:F13"/>
-    <mergeCell ref="G17:G18"/>
-    <mergeCell ref="B20:B21"/>
-    <mergeCell ref="C20:C21"/>
-    <mergeCell ref="D20:D21"/>
-    <mergeCell ref="E20:E21"/>
-    <mergeCell ref="F20:F21"/>
-    <mergeCell ref="G20:G21"/>
-    <mergeCell ref="B17:B18"/>
-    <mergeCell ref="C17:C18"/>
-    <mergeCell ref="D17:D18"/>
-    <mergeCell ref="E17:E18"/>
-    <mergeCell ref="F17:F18"/>
-    <mergeCell ref="G24:G25"/>
-    <mergeCell ref="B29:B30"/>
-    <mergeCell ref="C29:C30"/>
-    <mergeCell ref="D29:D30"/>
-    <mergeCell ref="E29:E30"/>
-    <mergeCell ref="F29:F30"/>
-    <mergeCell ref="G29:G30"/>
-    <mergeCell ref="B27:B28"/>
-    <mergeCell ref="C27:C28"/>
-    <mergeCell ref="D27:D28"/>
-    <mergeCell ref="E27:E28"/>
-    <mergeCell ref="F27:F28"/>
-    <mergeCell ref="G27:G28"/>
-    <mergeCell ref="B24:B25"/>
-    <mergeCell ref="C24:C25"/>
-    <mergeCell ref="D24:D25"/>
-    <mergeCell ref="E24:E25"/>
-    <mergeCell ref="F24:F25"/>
-    <mergeCell ref="B36:B37"/>
-    <mergeCell ref="C36:C37"/>
-    <mergeCell ref="D36:D37"/>
-    <mergeCell ref="E36:E37"/>
-    <mergeCell ref="F36:F37"/>
-    <mergeCell ref="G36:G37"/>
-    <mergeCell ref="G31:G32"/>
-    <mergeCell ref="B33:B34"/>
-    <mergeCell ref="C33:C34"/>
-    <mergeCell ref="D33:D34"/>
-    <mergeCell ref="E33:E34"/>
-    <mergeCell ref="F33:F34"/>
-    <mergeCell ref="G33:G34"/>
-    <mergeCell ref="B31:B32"/>
-    <mergeCell ref="C31:C32"/>
-    <mergeCell ref="D31:D32"/>
-    <mergeCell ref="E31:E32"/>
-    <mergeCell ref="F31:F32"/>
-    <mergeCell ref="B40:B41"/>
-    <mergeCell ref="C40:C41"/>
-    <mergeCell ref="D40:D41"/>
-    <mergeCell ref="E40:E41"/>
-    <mergeCell ref="F40:F41"/>
-    <mergeCell ref="G40:G41"/>
-    <mergeCell ref="B42:B43"/>
-    <mergeCell ref="C42:C43"/>
-    <mergeCell ref="D42:D43"/>
-    <mergeCell ref="E42:E43"/>
-    <mergeCell ref="F42:F43"/>
-    <mergeCell ref="G42:G43"/>
-    <mergeCell ref="B44:B45"/>
-    <mergeCell ref="C44:C45"/>
-    <mergeCell ref="D44:D45"/>
-    <mergeCell ref="E44:E45"/>
-    <mergeCell ref="F44:F45"/>
-    <mergeCell ref="G44:G45"/>
-    <mergeCell ref="G46:G47"/>
-    <mergeCell ref="B48:B49"/>
-    <mergeCell ref="C48:C49"/>
-    <mergeCell ref="D48:D49"/>
-    <mergeCell ref="E48:E49"/>
-    <mergeCell ref="F48:F49"/>
-    <mergeCell ref="G48:G49"/>
-    <mergeCell ref="B46:B47"/>
-    <mergeCell ref="C46:C47"/>
-    <mergeCell ref="D46:D47"/>
-    <mergeCell ref="E46:E47"/>
-    <mergeCell ref="F46:F47"/>
-    <mergeCell ref="G50:G51"/>
-    <mergeCell ref="B50:B51"/>
-    <mergeCell ref="C50:C51"/>
-    <mergeCell ref="D50:D51"/>
-    <mergeCell ref="E50:E51"/>
-    <mergeCell ref="F50:F51"/>
-    <mergeCell ref="G52:G53"/>
-    <mergeCell ref="B52:B53"/>
-    <mergeCell ref="C52:C53"/>
-    <mergeCell ref="D52:D53"/>
-    <mergeCell ref="E52:E53"/>
-    <mergeCell ref="F52:F53"/>
-    <mergeCell ref="G54:G55"/>
-    <mergeCell ref="B56:B57"/>
-    <mergeCell ref="C56:C57"/>
-    <mergeCell ref="D56:D57"/>
-    <mergeCell ref="E56:E57"/>
-    <mergeCell ref="F56:F57"/>
-    <mergeCell ref="G56:G57"/>
-    <mergeCell ref="B54:B55"/>
-    <mergeCell ref="C54:C55"/>
-    <mergeCell ref="D54:D55"/>
-    <mergeCell ref="E54:E55"/>
-    <mergeCell ref="F54:F55"/>
-    <mergeCell ref="G58:G59"/>
-    <mergeCell ref="B61:B62"/>
-    <mergeCell ref="C61:C62"/>
-    <mergeCell ref="D61:D62"/>
-    <mergeCell ref="E61:E62"/>
-    <mergeCell ref="F61:F62"/>
-    <mergeCell ref="G61:G62"/>
-    <mergeCell ref="B58:B59"/>
-    <mergeCell ref="C58:C59"/>
-    <mergeCell ref="D58:D59"/>
-    <mergeCell ref="E58:E59"/>
-    <mergeCell ref="F58:F59"/>
-    <mergeCell ref="G63:G64"/>
-    <mergeCell ref="B65:B66"/>
-    <mergeCell ref="C65:C66"/>
-    <mergeCell ref="D65:D66"/>
-    <mergeCell ref="E65:E66"/>
-    <mergeCell ref="F65:F66"/>
-    <mergeCell ref="G65:G66"/>
-    <mergeCell ref="B63:B64"/>
-    <mergeCell ref="C63:C64"/>
-    <mergeCell ref="D63:D64"/>
-    <mergeCell ref="E63:E64"/>
-    <mergeCell ref="F63:F64"/>
-    <mergeCell ref="G67:G68"/>
-    <mergeCell ref="B69:B70"/>
-    <mergeCell ref="C69:C70"/>
-    <mergeCell ref="D69:D70"/>
-    <mergeCell ref="E69:E70"/>
-    <mergeCell ref="F69:F70"/>
-    <mergeCell ref="G69:G70"/>
-    <mergeCell ref="B67:B68"/>
-    <mergeCell ref="C67:C68"/>
-    <mergeCell ref="D67:D68"/>
-    <mergeCell ref="E67:E68"/>
-    <mergeCell ref="F67:F68"/>
   </mergeCells>
-  <conditionalFormatting sqref="I6:I70">
+  <conditionalFormatting sqref="I6:I69">
     <cfRule type="expression" dxfId="0" priority="1">
       <formula>$I6=TRUE</formula>
     </cfRule>

</xml_diff>